<commit_message>
Latest code updating for framework
</commit_message>
<xml_diff>
--- a/TuduApplication/TestData/Registration.xlsx
+++ b/TuduApplication/TestData/Registration.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vikesh\Vikesh_eclipse\TuduApplication\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vikesh\git\MYtudu\TuduApplication\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1529CC32-5357-426B-B8C7-8AC7EEFD3089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85B096E-1A12-48C4-A27C-F31471AB2761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{E7554D94-690C-4CD3-9D75-8B2892EC350D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{E7554D94-690C-4CD3-9D75-8B2892EC350D}"/>
   </bookViews>
   <sheets>
     <sheet name="RegisterData" sheetId="1" r:id="rId1"/>
@@ -140,9 +140,6 @@
     <t>Doing testing to create project</t>
   </si>
   <si>
-    <t>aaa</t>
-  </si>
-  <si>
     <t>Account</t>
   </si>
   <si>
@@ -153,6 +150,9 @@
   </si>
   <si>
     <t>salma.vakil@aimdek.com</t>
+  </si>
+  <si>
+    <t>abc</t>
   </si>
 </sst>
 </file>
@@ -622,7 +622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911ED248-C567-496B-BA42-774C77C616F1}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -635,15 +635,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>13</v>
@@ -746,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A99F17E7-6350-4D09-A713-4B99FD160515}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,10 +780,10 @@
         <v>32</v>
       </c>
       <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
         <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>